<commit_message>
Filters added and ready for testing
</commit_message>
<xml_diff>
--- a/Projects/RINIELSENUS/Data/Template_2018.xlsx
+++ b/Projects/RINIELSENUS/Data/Template_2018.xlsx
@@ -36,9 +36,11 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hierarchy!$A$1:$K$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Hierarchy!$A$1:$K$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Hierarchy!$A$1:$K$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Hierarchy!$A$1:$K$144</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">sales!$A$1:$E$71</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">sales!$A$1:$E$71</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">sales!$A$1:$E$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">sales!$A$1:$E$71</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_FilterDatabase_0" vbProcedure="false">Anchor!$A$1:$N$11</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Anchor!$A$1:$N$11</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0" vbProcedure="false">Block!$A$1:$Q$46</definedName>
@@ -52,6 +54,7 @@
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Block!$A$1:$Q$46</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Block!$A$1:$Q$46</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Block!$A$1:$Q$46</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Block!$A$1:$Q$46</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_FilterDatabase_0" vbProcedure="false">Adjacency!$A$1:$S$21</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_FilterDatabase_0_0" vbProcedure="false">Adjacency!$A$1:$S$21</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_FilterDatabase_0_0_0" vbProcedure="false">Adjacency!$A$1:$S$21</definedName>
@@ -63,9 +66,11 @@
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">Adjacency!$A$1:$S$21</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">Adjacency!$A$1:$S$21</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Adjacency!$A$1:$S$21</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Adjacency!$A$1:$S$21</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">'Linear fair share'!$A$1:$I$22</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Linear fair share'!$A$1:$I$22</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Linear fair share'!$A$1:$I$22</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Linear fair share'!$A$1:$I$22</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2532,17 +2537,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="59.0242914979757"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="79.3765182186235"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="59.4493927125506"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.0161943319838"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="45.8461538461538"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.92712550607287"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="41.668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="41.9919028340081"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -6885,14 +6890,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="44.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="45.2024291497976"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.10526315789474"/>
   </cols>
@@ -7395,11 +7400,11 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="70.7004048582996"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="71.2348178137652"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7517,7 +7522,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.49797570850202"/>
@@ -7570,18 +7575,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="65.9838056680162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="66.5222672064777"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.03238866396761"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="7.92712550607287"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="91.587044534413"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="92.336032388664"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="6"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="9.10526315789474"/>
   </cols>
@@ -7678,12 +7683,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.3805668016194"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.7044534412956"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="9.10526315789474"/>
   </cols>
@@ -7758,9 +7763,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7866,7 +7871,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.2388663967611"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6"/>
@@ -7929,14 +7934,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
@@ -9055,18 +9060,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="57.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="57.8461538461538"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="44.0242914979757"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="39.3117408906883"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="44.3481781376518"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="39.6356275303644"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="6"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="9.10526315789474"/>
@@ -9450,10 +9455,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="63.5222672064777"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="64.0566801619433"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.0323886639676"/>
@@ -9535,14 +9540,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="78.9473684210526"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="79.6963562753036"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.10526315789474"/>
   </cols>
@@ -9985,12 +9990,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="30" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="30" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="30" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="30" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="30" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="30" width="26.7813765182186"/>
     <col collapsed="false" hidden="false" max="1023" min="7" style="30" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.57085020242915"/>
   </cols>
@@ -44287,26 +44292,26 @@
   </sheetPr>
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L47" activeCellId="0" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="67.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="67.7004048582996"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="32.0283400809717"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="44.0242914979757"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="14" min="12" style="1" width="41.8825910931174"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="44.3481781376518"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="14" min="12" style="1" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="1" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="9.10526315789474"/>
   </cols>
@@ -44387,7 +44392,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M2" s="30" t="s">
         <v>42</v>
@@ -44426,7 +44431,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M3" s="0"/>
       <c r="N3" s="4" t="s">
@@ -44463,7 +44468,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M4" s="30"/>
       <c r="N4" s="4" t="s">
@@ -44500,7 +44505,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M5" s="30"/>
       <c r="N5" s="4" t="s">
@@ -44537,7 +44542,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M6" s="30"/>
       <c r="N6" s="4" t="s">
@@ -44574,7 +44579,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M7" s="30"/>
       <c r="N7" s="4" t="s">
@@ -44611,7 +44616,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4" t="s">
@@ -44646,7 +44651,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
@@ -44681,7 +44686,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -44716,7 +44721,7 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
@@ -44751,7 +44756,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
@@ -44786,7 +44791,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>42</v>
@@ -44825,7 +44830,7 @@
       </c>
       <c r="K14" s="24"/>
       <c r="L14" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M14" s="24"/>
       <c r="N14" s="24"/>
@@ -44858,7 +44863,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
@@ -44893,7 +44898,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -44930,7 +44935,7 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
@@ -44967,7 +44972,7 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -45002,7 +45007,7 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
@@ -45039,7 +45044,7 @@
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
       <c r="L20" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M20" s="24"/>
       <c r="N20" s="24"/>
@@ -45072,7 +45077,7 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -45109,7 +45114,7 @@
       <c r="J22" s="24"/>
       <c r="K22" s="24"/>
       <c r="L22" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M22" s="24"/>
       <c r="N22" s="24"/>
@@ -45146,7 +45151,7 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
@@ -45183,7 +45188,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
@@ -45220,7 +45225,7 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
@@ -45257,7 +45262,7 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
@@ -45292,7 +45297,7 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M27" s="4" t="s">
         <v>42</v>
@@ -45329,7 +45334,7 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
@@ -45364,7 +45369,7 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
@@ -45399,7 +45404,7 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
@@ -45436,7 +45441,7 @@
       </c>
       <c r="K31" s="24"/>
       <c r="L31" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M31" s="24"/>
       <c r="N31" s="24"/>
@@ -45473,7 +45478,7 @@
       </c>
       <c r="K32" s="24"/>
       <c r="L32" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M32" s="24"/>
       <c r="N32" s="24"/>
@@ -45510,7 +45515,7 @@
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
@@ -45547,7 +45552,7 @@
         <v>585</v>
       </c>
       <c r="L34" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M34" s="24"/>
       <c r="N34" s="24"/>
@@ -45584,7 +45589,7 @@
         <v>586</v>
       </c>
       <c r="L35" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M35" s="24"/>
       <c r="N35" s="24"/>
@@ -45621,7 +45626,7 @@
         <v>587</v>
       </c>
       <c r="L36" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M36" s="24"/>
       <c r="N36" s="24"/>
@@ -45656,7 +45661,7 @@
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
@@ -45689,7 +45694,7 @@
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M38" s="4" t="s">
         <v>42</v>
@@ -45724,7 +45729,7 @@
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
@@ -45761,7 +45766,7 @@
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
@@ -45798,7 +45803,7 @@
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
@@ -45835,7 +45840,7 @@
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
@@ -45872,7 +45877,7 @@
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
@@ -45909,7 +45914,7 @@
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
@@ -45944,7 +45949,7 @@
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
       <c r="L45" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
@@ -45973,7 +45978,7 @@
         <v>589</v>
       </c>
       <c r="L46" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O46" s="28" t="s">
         <v>42</v>
@@ -46008,22 +46013,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="79.3765182186235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="80.0161943319838"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="41.8825910931174"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="1" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="19" min="18" style="1" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1022" min="20" style="1" width="9.10526315789474"/>
@@ -46951,8 +46956,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="34.5991902834008"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="34.8137651821862"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.497975708502"/>
@@ -46961,7 +46966,7 @@
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.03238866396761"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="32.5627530364372"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="9.10526315789474"/>
   </cols>

</xml_diff>